<commit_message>
fit soil, 3d nc read
</commit_message>
<xml_diff>
--- a/src/Input_data-default (synthetic).xlsx
+++ b/src/Input_data-default (synthetic).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\demostrator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA93C53-55C2-48E0-83BD-74814FEDF650}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D734578F-510E-4437-9808-9F3F8B8456CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2952" yWindow="2364" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="253">
   <si>
     <t>wlmin</t>
   </si>
@@ -835,6 +835,9 @@
   </si>
   <si>
     <t>synthetic</t>
+  </si>
+  <si>
+    <t>synthetic_sat</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2453,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2525,7 +2528,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D5" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
nc: working with single values, quality flags, coordinates alteration x-lat or x-lon does not matter, central pixel outside image check
</commit_message>
<xml_diff>
--- a/src/Input_data-default (synthetic).xlsx
+++ b/src/Input_data-default (synthetic).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\demostrator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D734578F-510E-4437-9808-9F3F8B8456CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BD34BA-3108-4927-9EF0-DD9174CB4D42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="260">
   <si>
     <t>wlmin</t>
   </si>
@@ -546,9 +546,6 @@
     <t>solar azimuth angle</t>
   </si>
   <si>
-    <t>band name</t>
-  </si>
-  <si>
     <t>observation azimuth angle</t>
   </si>
   <si>
@@ -564,9 +561,6 @@
     <t>pix_lon</t>
   </si>
   <si>
-    <t>(8, 3)</t>
-  </si>
-  <si>
     <t>image_path</t>
   </si>
   <si>
@@ -597,9 +591,6 @@
     <t>uneven (odd) integer or 0</t>
   </si>
   <si>
-    <t>Lae(47,4780833, 8,365)</t>
-  </si>
-  <si>
     <t>sun_zenith</t>
   </si>
   <si>
@@ -610,9 +601,6 @@
   </si>
   <si>
     <t>view_azimuth_mean</t>
-  </si>
-  <si>
-    <t>Maj (39,9415, -5,77336111)</t>
   </si>
   <si>
     <t>tz</t>
@@ -839,6 +827,121 @@
   <si>
     <t>synthetic_sat</t>
   </si>
+  <si>
+    <t>quality_flag_name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[OPTIONAL] band name: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>leave emtpy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if none</t>
+    </r>
+  </si>
+  <si>
+    <t>[OPTIONAL] band name: substituted by `tts` if absent</t>
+  </si>
+  <si>
+    <t>[OPTIONAL] band name: substituted by `tto` if absent</t>
+  </si>
+  <si>
+    <t>[OPTIONAL] band name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[OPTIONAL] band name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>required if K ~= 0</t>
+    </r>
+  </si>
+  <si>
+    <t>qulity flag</t>
+  </si>
+  <si>
+    <t>quality_flag_is</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[OPTIONAL] if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flag == quality_flag_is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fitting will be done for this pixel</t>
+    </r>
+  </si>
+  <si>
+    <t>quality_flag_lt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[OPTIONAL] if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flag &lt; quality_flag_ls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fitting will be done for this pixel</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -847,7 +950,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -871,6 +974,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1576,7 +1687,7 @@
         <v>0.4</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>71</v>
@@ -1856,7 +1967,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1894,10 +2005,10 @@
         <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1906,7 +2017,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1914,24 +2025,24 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1939,7 +2050,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
@@ -1950,7 +2061,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D7" t="s">
         <v>112</v>
@@ -1961,7 +2072,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C8" t="s">
         <v>104</v>
@@ -1975,7 +2086,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C9" t="s">
         <v>104</v>
@@ -1989,13 +2100,13 @@
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C10" t="s">
         <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2007,12 +2118,12 @@
         <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2026,10 +2137,10 @@
         <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2043,7 +2154,7 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2057,7 +2168,7 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2071,7 +2182,7 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2123,21 +2234,21 @@
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B24" s="10">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2165,7 +2276,7 @@
         <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2218,7 +2329,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2229,7 +2340,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2240,7 +2351,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2257,7 +2368,7 @@
         <v>51.540787999999999</v>
       </c>
       <c r="D35" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2268,49 +2379,49 @@
         <v>5.8602100000000004</v>
       </c>
       <c r="D36" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D37" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B38" s="10">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B39" s="10">
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D39" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2360,31 +2471,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" t="s">
         <v>216</v>
-      </c>
-      <c r="D2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2400,7 +2511,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2416,7 +2527,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2432,18 +2543,18 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2454,10 +2565,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2492,13 +2603,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2509,7 +2620,7 @@
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2517,7 +2628,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
         <v>106</v>
@@ -2528,7 +2639,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D5" t="s">
         <v>112</v>
@@ -2539,7 +2650,7 @@
         <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
         <v>104</v>
@@ -2553,7 +2664,7 @@
         <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
         <v>104</v>
@@ -2567,7 +2678,7 @@
         <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
         <v>105</v>
@@ -2585,7 +2696,7 @@
         <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2593,7 +2704,7 @@
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2601,13 +2712,13 @@
         <v>165</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
         <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2615,13 +2726,13 @@
         <v>166</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
         <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>171</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2629,13 +2740,13 @@
         <v>164</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
         <v>170</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2643,158 +2754,181 @@
         <v>167</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="D16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="B21" s="11">
+        <v>39.941499999999998</v>
+      </c>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B20" s="11">
-        <v>39.941499999999998</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" t="s">
-        <v>177</v>
-      </c>
-      <c r="E20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B21" s="10">
+      <c r="B22" s="10">
         <v>-5.7733611099999997</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B22" s="10">
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="10">
         <v>3</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D22" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="C23" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B24" s="10">
         <v>0.05</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="D26" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="10">
-        <v>44.8</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B29" s="10">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="10">
-        <v>19.7</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B30" s="10">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
         <v>98</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="10">
-        <v>223</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B31" s="10">
+        <v>154</v>
+      </c>
+      <c r="C31" t="s">
         <v>98</v>
       </c>
-      <c r="D28" t="s">
-        <v>184</v>
+      <c r="D31" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2808,7 +2942,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2821,36 +2955,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D1" t="s">
         <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
         <v>123</v>
       </c>
       <c r="G1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3293,7 +3427,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -3313,7 +3447,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>